<commit_message>
updated water isotopes, still not working
</commit_message>
<xml_diff>
--- a/data/sampling/water_iso/water_iso_data.xlsx
+++ b/data/sampling/water_iso/water_iso_data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/water_iso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/sampling/water_iso/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27455D0A-0137-584F-9BC7-35F4751FD8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED993AC-4CD6-354B-BF3B-A907D63AC099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15200" yWindow="-21620" windowWidth="26840" windowHeight="15940" xr2:uid="{957DCEBA-3732-5949-A769-67FC92AE3BDD}"/>
+    <workbookView xWindow="-15200" yWindow="-21640" windowWidth="26840" windowHeight="15940" xr2:uid="{957DCEBA-3732-5949-A769-67FC92AE3BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="13">
-  <si>
-    <t>Stick</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="14">
   <si>
     <t>top_depth</t>
   </si>
@@ -75,6 +72,12 @@
   </si>
   <si>
     <t>230_4</t>
+  </si>
+  <si>
+    <t>dxs</t>
+  </si>
+  <si>
+    <t>stick</t>
   </si>
 </sst>
 </file>
@@ -462,56 +465,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB03B01-A9CE-D045-BFF2-F738BF7F5C9B}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
+      <c r="I1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <f>155.065+J2/100</f>
         <v>155.065</v>
       </c>
       <c r="D2">
-        <f>155.065+K2/100</f>
-        <v>155.065</v>
+        <v>155.07499999999999</v>
       </c>
       <c r="E2">
-        <f>155.065+L2/100</f>
-        <v>155.065</v>
+        <v>155.07</v>
       </c>
       <c r="F2">
         <v>-296.18</v>
@@ -528,22 +531,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:E25" si="0">155.065+J3/100</f>
-        <v>155.065</v>
+        <v>155.0761</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.08609999999999</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.08109999999999</v>
       </c>
       <c r="F3">
         <v>-295.74</v>
@@ -560,22 +560,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.0873</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.09729999999999</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.09229999999999</v>
       </c>
       <c r="F4">
         <v>-295.99</v>
@@ -592,22 +589,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.0984</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.10839999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.10339999999999</v>
       </c>
       <c r="F5">
         <v>-296.24</v>
@@ -624,22 +618,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1095</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.11949999999999</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.11449999999999</v>
       </c>
       <c r="F6">
         <v>-296.55</v>
@@ -656,22 +647,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1207</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.13069999999999</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.12569999999999</v>
       </c>
       <c r="F7">
         <v>-296.07</v>
@@ -688,22 +676,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1318</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.14179999999999</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.13679999999999</v>
       </c>
       <c r="F8">
         <v>-295.07</v>
@@ -720,22 +705,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1429</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.15289999999999</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.14789999999999</v>
       </c>
       <c r="F9">
         <v>-294.05</v>
@@ -752,22 +734,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.154</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.16399999999999</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.15899999999999</v>
       </c>
       <c r="F10">
         <v>-293.89999999999998</v>
@@ -781,22 +760,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1652</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.17519999999999</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.17019999999999</v>
       </c>
       <c r="F11">
         <v>-293.23</v>
@@ -813,22 +789,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1763</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.18629999999999</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.18129999999999</v>
       </c>
       <c r="F12">
         <v>-292.74</v>
@@ -845,22 +818,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1874</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.19739999999999</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.19239999999999</v>
       </c>
       <c r="F13">
         <v>-292.31</v>
@@ -877,22 +847,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.1986</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.20859999999999</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.20359999999999</v>
       </c>
       <c r="F14">
         <v>-292</v>
@@ -909,22 +876,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2097</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.21969999999999</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.21469999999999</v>
       </c>
       <c r="F15">
         <v>-291.5</v>
@@ -941,22 +905,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2208</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.23079999999999</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.22579999999999</v>
       </c>
       <c r="F16">
         <v>-291.57</v>
@@ -973,22 +934,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.232</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.24199999999999</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.23699999999999</v>
       </c>
       <c r="F17">
         <v>-291.52999999999997</v>
@@ -1005,22 +963,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2431</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.25309999999999</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.24809999999999</v>
       </c>
       <c r="F18">
         <v>-291.63</v>
@@ -1037,22 +992,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2542</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.26419999999999</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.25919999999999</v>
       </c>
       <c r="F19">
         <v>-291.66000000000003</v>
@@ -1069,22 +1021,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2653</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.27529999999999</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.27029999999999</v>
       </c>
       <c r="F20">
         <v>-291.20999999999998</v>
@@ -1101,22 +1050,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2765</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.28649999999999</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.28149999999999</v>
       </c>
       <c r="F21">
         <v>-290.92</v>
@@ -1133,22 +1079,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2876</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.29759999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.29259999999999</v>
       </c>
       <c r="F22">
         <v>-291.08</v>
@@ -1165,22 +1108,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.2987</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.30869999999999</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.30369999999999</v>
       </c>
       <c r="F23">
         <v>-292</v>
@@ -1197,22 +1137,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.3099</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.31989999999999</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.31489999999999</v>
       </c>
       <c r="F24">
         <v>-293.97000000000003</v>
@@ -1229,22 +1166,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.321</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.33799999999999</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>155.065</v>
+        <v>155.3295</v>
       </c>
       <c r="F25">
         <v>-294.24</v>
@@ -1261,22 +1195,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <f>155.065+(J26+1.3)/100</f>
         <v>155.078</v>
       </c>
       <c r="D26">
-        <f>155.065+(K26+1.3)/100</f>
-        <v>155.078</v>
+        <v>155.08799999999999</v>
       </c>
       <c r="E26">
-        <f>155.065+(L26+1.3)/100</f>
-        <v>155.078</v>
+        <v>155.083</v>
       </c>
       <c r="F26">
         <v>-291.11</v>
@@ -1293,22 +1224,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:E46" si="1">155.065+(J27+1.3)/100</f>
-        <v>155.078</v>
+        <v>155.0891</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.09909999999999</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.0941</v>
       </c>
       <c r="F27">
         <v>-291.67</v>
@@ -1325,22 +1253,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1001</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.11009999999999</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.10509999999999</v>
       </c>
       <c r="F28">
         <v>-291.60000000000002</v>
@@ -1357,22 +1282,19 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1112</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.12119999999999</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.11619999999999</v>
       </c>
       <c r="F29">
         <v>-291.25</v>
@@ -1389,22 +1311,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.12219999999999</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.13220000000001</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.12719999999999</v>
       </c>
       <c r="F30">
         <v>-291.13</v>
@@ -1421,22 +1340,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.13329999999999</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.14330000000001</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.13829999999999</v>
       </c>
       <c r="F31">
         <v>-290.97000000000003</v>
@@ -1453,22 +1369,19 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.14429999999999</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.15430000000001</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.14930000000001</v>
       </c>
       <c r="F32">
         <v>-291.77</v>
@@ -1485,22 +1398,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.15539999999999</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.16540000000001</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.16040000000001</v>
       </c>
       <c r="F33">
         <v>-291.29000000000002</v>
@@ -1517,22 +1427,19 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.16640000000001</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1764</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.17140000000001</v>
       </c>
       <c r="F34">
         <v>-291.16000000000003</v>
@@ -1549,22 +1456,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.17750000000001</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1875</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1825</v>
       </c>
       <c r="F35">
         <v>-291.08999999999997</v>
@@ -1581,22 +1485,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1885</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1985</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1935</v>
       </c>
       <c r="F36">
         <v>-290.52999999999997</v>
@@ -1613,22 +1514,19 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.1996</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.20959999999999</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.2046</v>
       </c>
       <c r="F37">
         <v>-290.19</v>
@@ -1645,22 +1543,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.2106</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.22059999999999</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.21559999999999</v>
       </c>
       <c r="F38">
         <v>-290.24</v>
@@ -1677,22 +1572,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.2217</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.23169999999999</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.22669999999999</v>
       </c>
       <c r="F39">
         <v>-291.3</v>
@@ -1709,22 +1601,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.23269999999999</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.24269999999999</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.23769999999999</v>
       </c>
       <c r="F40">
         <v>-292.87</v>
@@ -1738,22 +1627,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.24379999999999</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.25379999999998</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.24879999999999</v>
       </c>
       <c r="F41">
         <v>-294.63</v>
@@ -1770,22 +1656,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.25479999999999</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.26480000000001</v>
       </c>
       <c r="E42">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.25979999999998</v>
       </c>
       <c r="F42">
         <v>-295.45</v>
@@ -1802,22 +1685,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.26589999999999</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.27590000000001</v>
       </c>
       <c r="E43">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.27090000000001</v>
       </c>
       <c r="F43">
         <v>-296.16000000000003</v>
@@ -1834,22 +1714,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.27690000000001</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.2869</v>
       </c>
       <c r="E44">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.28190000000001</v>
       </c>
       <c r="F44">
         <v>-296.13</v>
@@ -1866,22 +1743,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.28800000000001</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.298</v>
       </c>
       <c r="E45">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.29300000000001</v>
       </c>
       <c r="F45">
         <v>-295.7</v>
@@ -1898,22 +1772,19 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.29900000000001</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.316</v>
       </c>
       <c r="E46">
-        <f t="shared" si="1"/>
-        <v>155.078</v>
+        <v>155.3075</v>
       </c>
       <c r="F46">
         <v>-294.75</v>
@@ -1930,19 +1801,19 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C47">
+        <f>E47-0.005</f>
+        <v>155.065</v>
+      </c>
+      <c r="D47">
         <f>E47+0.005</f>
         <v>155.07499999999999</v>
       </c>
-      <c r="D47">
-        <f>E47-0.005</f>
-        <v>155.065</v>
-      </c>
       <c r="E47" s="1">
         <v>155.07</v>
       </c>
@@ -1958,10 +1829,18 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:C74" si="0">E48-0.005</f>
+        <v>155.07500000000002</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:D74" si="1">E48+0.005</f>
+        <v>155.08500000000001</v>
       </c>
       <c r="E48" s="1">
         <v>155.08000000000001</v>
@@ -1978,10 +1857,18 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>155.08500000000001</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>155.095</v>
       </c>
       <c r="E49" s="1">
         <v>155.09</v>
@@ -1998,10 +1885,18 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>155.095</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>155.10499999999999</v>
       </c>
       <c r="E50" s="1">
         <v>155.1</v>
@@ -2018,10 +1913,18 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>155.10500000000002</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>155.11500000000001</v>
       </c>
       <c r="E51" s="1">
         <v>155.11000000000001</v>
@@ -2038,10 +1941,18 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>155.11500000000001</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>155.125</v>
       </c>
       <c r="E52" s="1">
         <v>155.12</v>
@@ -2058,10 +1969,18 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>155.125</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>155.13499999999999</v>
       </c>
       <c r="E53" s="1">
         <v>155.13</v>
@@ -2078,10 +1997,18 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>155.13499999999999</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>155.14499999999998</v>
       </c>
       <c r="E54" s="1">
         <v>155.13999999999999</v>
@@ -2098,10 +2025,18 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>155.14500000000001</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>155.155</v>
       </c>
       <c r="E55" s="1">
         <v>155.15</v>
@@ -2118,10 +2053,18 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>155.155</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>155.16499999999999</v>
       </c>
       <c r="E56" s="1">
         <v>155.16</v>
@@ -2138,10 +2081,18 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>155.16499999999999</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>155.17499999999998</v>
       </c>
       <c r="E57" s="1">
         <v>155.16999999999999</v>
@@ -2158,10 +2109,18 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>155.17500000000001</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>155.185</v>
       </c>
       <c r="E58" s="1">
         <v>155.18</v>
@@ -2178,10 +2137,18 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>155.185</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>155.19499999999999</v>
       </c>
       <c r="E59" s="1">
         <v>155.19</v>
@@ -2198,10 +2165,18 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>155.19499999999999</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>155.20499999999998</v>
       </c>
       <c r="E60" s="1">
         <v>155.19999999999999</v>
@@ -2218,10 +2193,18 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>155.20500000000001</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>155.215</v>
       </c>
       <c r="E61" s="1">
         <v>155.21</v>
@@ -2238,10 +2221,18 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>155.215</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>155.22499999999999</v>
       </c>
       <c r="E62" s="1">
         <v>155.22</v>
@@ -2258,10 +2249,18 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>155.22499999999999</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>155.23499999999999</v>
       </c>
       <c r="E63" s="1">
         <v>155.22999999999999</v>
@@ -2278,10 +2277,18 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>155.23500000000001</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>155.245</v>
       </c>
       <c r="E64" s="1">
         <v>155.24</v>
@@ -2298,10 +2305,18 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>155.245</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>155.255</v>
       </c>
       <c r="E65" s="1">
         <v>155.25</v>
@@ -2318,10 +2333,18 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>155.255</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>155.26499999999999</v>
       </c>
       <c r="E66" s="1">
         <v>155.26</v>
@@ -2338,10 +2361,18 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>155.26500000000001</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="1"/>
+        <v>155.27500000000001</v>
       </c>
       <c r="E67" s="1">
         <v>155.27000000000001</v>
@@ -2358,10 +2389,18 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>155.27500000000001</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>155.285</v>
       </c>
       <c r="E68" s="1">
         <v>155.28</v>
@@ -2378,10 +2417,18 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>155.285</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>155.29499999999999</v>
       </c>
       <c r="E69" s="1">
         <v>155.29</v>
@@ -2398,10 +2445,18 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>155.29500000000002</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>155.30500000000001</v>
       </c>
       <c r="E70" s="1">
         <v>155.30000000000001</v>
@@ -2418,10 +2473,18 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="0"/>
+        <v>155.30500000000001</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>155.315</v>
       </c>
       <c r="E71" s="1">
         <v>155.31</v>
@@ -2438,10 +2501,18 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="0"/>
+        <v>155.315</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>155.32499999999999</v>
       </c>
       <c r="E72" s="1">
         <v>155.32</v>
@@ -2458,10 +2529,18 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="0"/>
+        <v>155.32500000000002</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>155.33500000000001</v>
       </c>
       <c r="E73" s="1">
         <v>155.33000000000001</v>
@@ -2478,10 +2557,18 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="0"/>
+        <v>155.33500000000001</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>155.345</v>
       </c>
       <c r="E74" s="1">
         <v>155.34</v>
@@ -2498,10 +2585,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75">
         <v>156.81</v>
@@ -2525,10 +2612,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76">
         <v>156.82499999999999</v>
@@ -2552,10 +2639,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77">
         <v>156.83699999999999</v>
@@ -2579,10 +2666,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C78">
         <v>156.84899999999999</v>
@@ -2606,10 +2693,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C79">
         <v>156.86199999999999</v>
@@ -2633,10 +2720,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C80">
         <v>156.874</v>
@@ -2660,10 +2747,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81">
         <v>156.886</v>
@@ -2687,10 +2774,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82">
         <v>156.898</v>
@@ -2714,10 +2801,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83">
         <v>156.91</v>
@@ -2741,10 +2828,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C84">
         <v>156.922</v>
@@ -2768,10 +2855,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C85">
         <v>156.935</v>
@@ -2795,10 +2882,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C86">
         <v>156.947</v>
@@ -2822,10 +2909,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87">
         <v>156.959</v>
@@ -2849,10 +2936,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C88">
         <v>156.971</v>
@@ -2876,10 +2963,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C89">
         <v>156.983</v>
@@ -2903,10 +2990,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C90">
         <v>156.995</v>
@@ -2930,10 +3017,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C91">
         <v>157.00800000000001</v>
@@ -2957,10 +3044,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C92">
         <v>157.02000000000001</v>
@@ -2984,10 +3071,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C93">
         <v>156.78700000000001</v>
@@ -3011,10 +3098,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94">
         <v>156.80699999999999</v>
@@ -3038,10 +3125,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95">
         <v>156.81899999999999</v>
@@ -3065,10 +3152,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C96">
         <v>156.83099999999999</v>
@@ -3092,10 +3179,10 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C97">
         <v>156.84299999999999</v>
@@ -3119,10 +3206,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98">
         <v>156.85499999999999</v>
@@ -3146,10 +3233,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C99">
         <v>156.86699999999999</v>
@@ -3173,10 +3260,10 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C100">
         <v>156.88300000000001</v>
@@ -3200,10 +3287,10 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C101">
         <v>156.89500000000001</v>
@@ -3227,10 +3314,10 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C102">
         <v>156.90700000000001</v>
@@ -3254,10 +3341,10 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C103">
         <v>156.91900000000001</v>
@@ -3281,10 +3368,10 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C104">
         <v>156.93100000000001</v>
@@ -3308,10 +3395,10 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C105">
         <v>156.94300000000001</v>
@@ -3335,10 +3422,10 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C106">
         <v>156.95500000000001</v>
@@ -3362,10 +3449,10 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C107">
         <v>156.96700000000001</v>
@@ -3389,10 +3476,10 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C108">
         <v>156.97900000000001</v>
@@ -3416,10 +3503,10 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C109">
         <v>156.99100000000001</v>
@@ -3443,10 +3530,10 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C110">
         <v>157.00299999999999</v>
@@ -3470,10 +3557,10 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C111">
         <v>157.01499999999999</v>

</xml_diff>